<commit_message>
Vanilla Races Expanded - Lycanthrope 업데이트
#296
</commit_message>
<xml_diff>
--- a/Data/Vanilla Expanded/Vanilla Races Expanded - Lycanthrope - 3114453100/3114453100.xlsx
+++ b/Data/Vanilla Expanded/Vanilla Races Expanded - Lycanthrope - 3114453100/3114453100.xlsx
@@ -8,14 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\RimWorld\Mods\RMK\Data\Vanilla Expanded\Vanilla Races Expanded - Lycanthrope - 3114453100\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77843452-974D-4853-94E0-12AB5550FFB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDC1462A-8EAF-40B1-B62B-924C072E1E6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7450" yWindow="0" windowWidth="30950" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Main" sheetId="1" r:id="rId1"/>
+    <sheet name="Main_231218" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -386,7 +399,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="638">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="791">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -2294,14 +2307,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>무리 동료 {0} 잃음</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>무리 동료 {0} 팔림</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>조건 변이: 야간</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2422,6 +2427,497 @@
   </si>
   <si>
     <t>특별한 주입 기관을 사용해서 이 사람의 생식유전자를 원하는 사람에게 이식합니다. 유전자가 재성장 중일 때 이 능력을 사용하면 변형이식체를 이식한 후 사망합니다.\n\n이식된 변형이식체는 대상의 생식유전자를 덮어씁니다. 변형인자는 영향받지 않습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>광 공포증 알림 비활성</t>
+  </si>
+  <si>
+    <t>기본적으로, 광 공포증을 가진 폰이 빛으로부터 달아날 때마다 게임은 플레이어에게 이를 알리는 편지를 생성합니다. 많은 폰이 자주 도망친다면 이것은 다소 짜증나며 게임 플레이에 영향이 있을 수 있으므로, 이 옵션으로 비활성화할 수 있습니다. 폰들이 여전히 도망친다는 것을 명심하십시오. 메세지를 받지 못할 뿐입니다.</t>
+  </si>
+  <si>
+    <t>{0_labelShort} has no available endogenes to implant.</t>
+  </si>
+  <si>
+    <t>변이</t>
+  </si>
+  <si>
+    <t>다른 인종형으로 변이합니다.</t>
+  </si>
+  <si>
+    <t>전투의 포효</t>
+  </si>
+  <si>
+    <t>주변에 있는 아군들의 전투력을 높이는 커다란 포효를 내지릅니다.</t>
+  </si>
+  <si>
+    <t>유전자 이식</t>
+  </si>
+  <si>
+    <t>이 사람의 유전자를 특별한 주입기 기관을 이용해 대상에게 이식합니다. 이 사람의 유전자가 현재 다시 재성장 중이라면, 그 과정에서 유전자를 이식하고 죽게 될 것입니다.\n\이식되면 생식선이 표적의 생식선을 덮어씁니다. 인종형 유전자는 영향을 받지 않을 것입니다.</t>
+  </si>
+  <si>
+    <t>앨리슨</t>
+  </si>
+  <si>
+    <t>바셋</t>
+  </si>
+  <si>
+    <t>빌</t>
+  </si>
+  <si>
+    <t>보스웰</t>
+  </si>
+  <si>
+    <t>헤이즈</t>
+  </si>
+  <si>
+    <t>히치콕</t>
+  </si>
+  <si>
+    <t>홀리데이</t>
+  </si>
+  <si>
+    <t>매터슨</t>
+  </si>
+  <si>
+    <t>모건</t>
+  </si>
+  <si>
+    <t>팻</t>
+  </si>
+  <si>
+    <t>버질</t>
+  </si>
+  <si>
+    <t>울프맨</t>
+  </si>
+  <si>
+    <t>울프맨 무리 입니다.</t>
+  </si>
+  <si>
+    <t>우두머리</t>
+  </si>
+  <si>
+    <t>근접 회피</t>
+  </si>
+  <si>
+    <t>이 유전자의 보유자는 아군의 사기를 드높이는 강렬한 포효를 사용할 수 있으며 아군들의 공세를 더욱 거세게 만들 수 있습니다.</t>
+  </si>
+  <si>
+    <t>전투 포효의 효과는 10회까지 중첩됩니다.</t>
+  </si>
+  <si>
+    <t>유전자 이식기관</t>
+  </si>
+  <si>
+    <t>이 유전자의 보유자는 유전자 주입 기관을 통해 자신의 생식유전자를 다른 사람에게 이식할 수 있습니다. 그 후 자신의 유전자는 매우 천천히 재생합니다. 만약 재생되는 동안 다시 이식한다면 죽을 것입니다.</t>
+  </si>
+  <si>
+    <t>가슴털</t>
+  </si>
+  <si>
+    <t>이 유전자의 보유자는 가슴에 두터운 털이 자라게 됩니다.</t>
+  </si>
+  <si>
+    <t>대화 불가능</t>
+  </si>
+  <si>
+    <t>이 유전자의보유자는 대화의 과정에서 듣고 이해하고 말하는 능력을 잃었습니다.</t>
+  </si>
+  <si>
+    <t>뾰족한 귀</t>
+  </si>
+  <si>
+    <t>이 유전자의 보유자는 늑대와 같은 귀를 가지게 됩니다.</t>
+  </si>
+  <si>
+    <t>뾰족한 코</t>
+  </si>
+  <si>
+    <t>이 유전자의 보유자는 늑대와 같은 코를 가지게 됩니다.</t>
+  </si>
+  <si>
+    <t>늑대의 꼬리</t>
+  </si>
+  <si>
+    <t>이 유전자의 보유자는 늑대처럼 생긴 꼬리가 자라나며 움직임을 약간 돕습니다.</t>
+  </si>
+  <si>
+    <t>구레나룻</t>
+  </si>
+  <si>
+    <t>이 유전자의 남성 보유자들은 얼굴 측면에 엄청난 속도로 수염이 자랍니다 .</t>
+  </si>
+  <si>
+    <t>뛰어난 어둠속 시야</t>
+  </si>
+  <si>
+    <t>이 유전자의 보유자는 빛이 잘 드는 지역보다 어둠속을 훨씬 더 잘 볼 수 있으며, 어둠과 관련된 기분 불이익에 영향을 받지 않습니다. 망막 뒤에 어둠 속에서 보는 능력을 증폭시키는 반사층을 가지고 있습니다.</t>
+  </si>
+  <si>
+    <t>광 민감성</t>
+  </si>
+  <si>
+    <t>이 유전자의 보유자는 눈에 생물학적 화합물을 가지고 있는데, 이 화합물은 빛의 광자에 고통스럽게 반응합니다. 그들은 어떤 광원에도 매우 민감합니다.</t>
+  </si>
+  <si>
+    <t>극심한 광 민감성</t>
+  </si>
+  <si>
+    <t>이 유전자의 보유자는 눈에 빛 광자에 위험하게 반응하는 생물학적 화합물을 가지고 있습니다. 그들은 어떤 광원에도 비정상적으로 민감합니다.</t>
+  </si>
+  <si>
+    <t>향산된 회피력</t>
+  </si>
+  <si>
+    <t>이 유전자의 보유자는 공격을 더 쉽게 피할 수 있습니다. 인지 능력이 뛰어나기 때문에 공격이 일어나기 전에 이미 알고 있습니다.</t>
+  </si>
+  <si>
+    <t>뛰어난 회피력</t>
+  </si>
+  <si>
+    <t>이 유전자의 운반체는 공격을 매우 쉽게 피할 수 있습니다. 인지 능력이 뛰어나기 때문에, 그들은 공격이 본능적으로 피해집니다.</t>
+  </si>
+  <si>
+    <t>회피 불가</t>
+  </si>
+  <si>
+    <t>이 유전자의 보유자는 공격을 피할 수 없습니다. 전투 인식이 부족하면 모든 스윙에 맞습니다. 심지어 놓치는 스윙에도 맞습니다.</t>
+  </si>
+  <si>
+    <t>광 공포증</t>
+  </si>
+  <si>
+    <t>이 유전자의 보유자는 빛에 대한 강렬한 공포를 가지고 있습니다. 어떤 광원이라도 가까이 있으면 언제든지 상태이상에 빠질 가능성이 있습니다.</t>
+  </si>
+  <si>
+    <t>무리의 사고방식</t>
+  </si>
+  <si>
+    <t>이 유전자의 보유자는 끈끈하게 이어진 공동체를 형성할 수 있으며, 그들의 공동체가 크고 강할수록 더 행복해집니다.</t>
+  </si>
+  <si>
+    <t>영역 중시</t>
+  </si>
+  <si>
+    <t>이 유전자의 보유자는 극도로 영역을 중요시합니다, 자신의 영역에선 정신적으로 안정되지만, 영역에서 벗어나면 정식적으로 불안해집니다.</t>
+  </si>
+  <si>
+    <t>변이: 야간</t>
+  </si>
+  <si>
+    <t>이 유전자의 보유자는 밤마다 변이를 겪습니다. 변이를 멈추거나 방지할 수 있는 방법은 없으며, 아침이 되면 되돌아옵니다.</t>
+  </si>
+  <si>
+    <t>변이: 성장</t>
+  </si>
+  <si>
+    <t>이 유전자의 보유자는 성인이 되면 변이를 겪습니다. 변이를 멈추거나 방지할 수 있는 방법은 없으며, 한 번 변이하면 되돌아 올 수 없습니다.</t>
+  </si>
+  <si>
+    <t>변이: 계절</t>
+  </si>
+  <si>
+    <t>이 유전자의 보유자는 3분기(가을)가 되면 변이를 겪으며, 1분기(봄)가 되면 다시 되돌아옵니다.</t>
+  </si>
+  <si>
+    <t>변이: 부상</t>
+  </si>
+  <si>
+    <t>이 유전자의 보유자는 심하게 부상 당했을 때 변이를 겪고, 거의 완전히 회복되었을 때에만 되돌아 옵니다.</t>
+  </si>
+  <si>
+    <t>변이: 돌발</t>
+  </si>
+  <si>
+    <t>이 유전자의 보유자는 무작위적인 변이를 겪습니다. 변이가 일어나는 조건이나 제어할 수 있는 방법은 아무도 알지 못합니다.</t>
+  </si>
+  <si>
+    <t>야행성</t>
+  </si>
+  <si>
+    <t>이 유전자의 보유자는 밤에 일하는 것을 선호합니다. 밤에 깨어 있으면 더 행복해지고 낮에 깨어 있으면 불행해집니다.</t>
+  </si>
+  <si>
+    <t>극도로 빠른 발걸음</t>
+  </si>
+  <si>
+    <t>이 유전자의 보유자는 인간을 초월한 속도로 움직일 수 있도록 하는 특수한 근육 자극 세포를 가지고 있습니다.</t>
+  </si>
+  <si>
+    <t>지형에 따른 이동속도 감소를 무시합니다.</t>
+  </si>
+  <si>
+    <t>엄청나게 빠름</t>
+  </si>
+  <si>
+    <t>이 사람은 매우 빠르게 움직입니다. 그들은 이동할 때 지형에 따른 보행속도 불이익을 무시할 것입니다.</t>
+  </si>
+  <si>
+    <t>전투의 포효 능력으로 인한 전투력 증가. 최대 10회 중첩되며 3시간 지속됨.</t>
+  </si>
+  <si>
+    <t>생식 유전자 이식 혼수상태</t>
+  </si>
+  <si>
+    <t>이 사람에게 생식유전자를 이식했습니다. 생식 유전자는 숙주와 통합하고 몸 전체에 있는 다양한 유전자와 화학적 성질을 바꾸는 데 시간이 필요합니다. 이 시간 동안 사람은 깨어날 수 없기 때문에 생식 유전자은 그들을 혼수상태로 유지합니다.\n\더 나은 의료 시설과 더 숙련된 의사가 생식 유전자를 이식함으로써 이 혼수상태의 기간을 줄일 수 있습니다.</t>
+  </si>
+  <si>
+    <t>생식유전자 추출 충격</t>
+  </si>
+  <si>
+    <t>이 사람의 생식유전자는 최근에 제거되거나 추출되었습니다. 이것은 그 사람의 신진대사와 호르몬을 불안정하게 하여 일시적으로 약하고 나른한 상태를 유지하고 면역체계를 약화시킵니다.</t>
+  </si>
+  <si>
+    <t>대상에게서 생식유전자 추출.</t>
+  </si>
+  <si>
+    <t>빛을 두려워함</t>
+  </si>
+  <si>
+    <t>빛에게서 도망치는 중</t>
+  </si>
+  <si>
+    <t>빛을 피하는중</t>
+  </si>
+  <si>
+    <t>{0}(이)가 빛으로부터 도망치고 있습니다.</t>
+  </si>
+  <si>
+    <t>{0}(은)는 더 이상 빛을 피하지 않습니다.</t>
+  </si>
+  <si>
+    <t>상태: 빛으로부터 도망침</t>
+  </si>
+  <si>
+    <t>무리원</t>
+  </si>
+  <si>
+    <t>shipAdjective-&gt;울프맨</t>
+  </si>
+  <si>
+    <t>shipAdjective-&gt;늑대의</t>
+  </si>
+  <si>
+    <t>shipAdjective-&gt;라이칸</t>
+  </si>
+  <si>
+    <t>shipAdjective-&gt;웨어울프</t>
+  </si>
+  <si>
+    <t>shipAdjective-&gt;한밤의</t>
+  </si>
+  <si>
+    <t>shipAdjective-&gt;울부짖음</t>
+  </si>
+  <si>
+    <t>shipAdjective-&gt;털복숭이</t>
+  </si>
+  <si>
+    <t>shipAdjective-&gt;송곳니의</t>
+  </si>
+  <si>
+    <t>shipNoun-&gt;함선</t>
+  </si>
+  <si>
+    <t>shipNoun-&gt;왕복선</t>
+  </si>
+  <si>
+    <t>shipNoun-&gt;선박</t>
+  </si>
+  <si>
+    <t>shipNoun-&gt;폐선박</t>
+  </si>
+  <si>
+    <t>shipNoun-&gt;불시착</t>
+  </si>
+  <si>
+    <t>shipNoun-&gt;잔해</t>
+  </si>
+  <si>
+    <t>questDescription-&gt;당신은 다급한 구조요청을 받았습니다! 울프맨 난민들을 태운 왕복선이 운항중 문제가 생겼습니다. 그들의 지도자와, 그를 포함한 [WolfmenCount] 다른 난민들은 그들이 근처에 불시착하는 것을 허락해달라고 당신에게 간청하고 있습니다. \n\n일단 그 배가 불시착하면, 울프맨들은 다시 무리를 지어 지역을 떠날 것입니다. 만약 당신이 그들이 당신의 근처에 불시착하도록 허락한다면, 그들은 당신의 정착지지 주민들 중 한 명을 울프맨으로 바꿔주겠다고 제안합니다. 당신은 또한 이 기회를 그들과 싸우거나 체포하는데 사용할 수 있습니다. 당신이 그들 중 한 명을 포획할 수 있다면, 당신은 그들을 당신의 식민지 주민 중 한 명을 울프맨으로 바꾸도록 강제할 수 있습니다.\n\n[wolfmenInfo]</t>
+  </si>
+  <si>
+    <t>wolfmenInfo-&gt;(*Gray)울프맨에 대해: 울프맨은 더 많은 영토의 소유권을 주장하고 무리 또는 더 큰 씨족을 형성하기 위해 변방계 곳곳으로 전파 되었습니다. 그들의 울프맨 형태는 그들의 야행성 능력을 감소시킵니다, 이 형태에선 그들의 인종형을 다른 사람들에게 공유할수 있지만 변신했을 때 보다는 이점이 낮습니다. 반면, 그들의 라이칸 형태는 야행성의 이점, 향상된 근접 전투 효율성, 초자연적인 속도 및 재생, 그리고 더 많은 무리의 인원들이 합류함에 따라 더욱 강해지는 전투의 함성 능력을 가지게 됩니다.(/Gray)</t>
+  </si>
+  <si>
+    <t>wolfmanShuttleCrashedLetterLabel-&gt;불시착한 왕복선</t>
+  </si>
+  <si>
+    <t>wolfmanShuttleCrashedLetterText-&gt;울프맨 우두머리와 [WolfmenCount] 울프맨 난민들이 탑승한 왕복선이 근처에 불시착 했습니다. 그들은 불시착한 우주선을 빠져나와 지역을 떠날 준비를 할 것입니다.</t>
+  </si>
+  <si>
+    <t>reinforcementsArrivedLetterLabel-&gt;울프맨 증원군</t>
+  </si>
+  <si>
+    <t>reinforcementsArrivedLetterText-&gt;울프맨들이 추락한 피난민들을 지원하기 위해 수송 포드를 타고 도착하고 있습니다.</t>
+  </si>
+  <si>
+    <t>letterLabelBeggarsBetrayed-&gt;배신당한 난민</t>
+  </si>
+  <si>
+    <t>letterTextBeggarsBetrayed-&gt;울프맨 난민들은 당신에게 배신당했으며 최대한 자신들을 보호하려고 할 것입니다.</t>
+  </si>
+  <si>
+    <t>빛은 불쾌해, 눈을 아프게 만들어.</t>
+  </si>
+  <si>
+    <t>극심한 광민감성</t>
+  </si>
+  <si>
+    <t>여기는 빛이 너무 많아, 눈이 아프다고!</t>
+  </si>
+  <si>
+    <t>그 빛은 나를 너무 불안하게 만들어. 마치 나를 불태워버리는 것만 같아!</t>
+  </si>
+  <si>
+    <t>무리원 {0} 사망</t>
+  </si>
+  <si>
+    <t>.우리 무리원이 죽었어. 무리가 약해질거야.</t>
+  </si>
+  <si>
+    <t>무리원 {0} 실종</t>
+  </si>
+  <si>
+    <t>우리는 소중한 무리원중 한명을 잃었어. 그들이 무리가 없이 살아남을 수 있을까?</t>
+  </si>
+  <si>
+    <t>무리원 살해</t>
+  </si>
+  <si>
+    <t>무리원 {0} 팔아넘김</t>
+  </si>
+  <si>
+    <t>무리원을 팔아넘김</t>
+  </si>
+  <si>
+    <t>우리는 방금 막 무리원을 팔아넘겼어, 이러고도 우리를 무리라고 부를 수 있을까?</t>
+  </si>
+  <si>
+    <t>우리의 무리는 더 강해지고 있어. 무리가 클수록 우리는 더 안정감을 느껴.</t>
+  </si>
+  <si>
+    <t>변이: {0}</t>
+  </si>
+  <si>
+    <t>이 유전자의 보유자는 빠르게 다른 형태로 변이하는 비범한 능력을 가지고 있습니다 {0} 그들은 그 인종형의 모든 능력과 단점을 물려받으며, 조건만 맞다면 다시 형태를 바꿀 수 있을 것입니다.</t>
+  </si>
+  <si>
+    <t>울프맨/라이칸은 기원이 불분명한 인종형으로, 영토를 확장하며 무리 또는 더 큰 씨족을 형성하기 위해 변방계 곳곳에 전파되었습니다. 그들의 울프맨 형태는 야행성 능력을 감소시키고, 그들의 유전자를 다른 사람들과 공유할 수 있는 대가로 많은 이점을 포기했습니다.\n\n라이칸의 역사에 대해 확립된 명확한 역사는 없으며, 특히 그들의 무리는 자신의 기원을 조작하는 경향이 있기 때문에 더욱 모호합니다. 이것은 매우 다양한 음모론으로 이어졌으며, 특히 유전자의 유사성 때문에 많은 사람들이 부분적으로라도 생귀오파지와 관련이 있다고 생각합니다. 가장 일반적인 가설은 생귀오파지가 이타킨과 사랑에 빠졌고, 나중에 그들의 아이가 변이되었다는 것이지만, 또 다른 이야기에선 생귀오파지가 임신한 후 여러 복잡한 문제가 덮쳐왔고. 아이는 태어났지만 부모에게 버림받았으며 길 잃은 개들 사이에서 길러졌다는 것 입니다. 결국 그들은 혈육보다 끈끈한 유대로 자신의 가족을 만들었고, 가족이 최우선 이라는 것을 항상 마음에 새겼다는 것입니다.</t>
+  </si>
+  <si>
+    <t>라이칸</t>
+  </si>
+  <si>
+    <t>울프맨/라이칸은 기원이 불분명한 인종형으로, 영토를 확장하며 무리 또는 더 큰 씨족을 형성하기 위해 변방계 곳곳에 전파되었습니다. 그들의 라이칸 형태는 야행성의 이점, 향상된 근접 전투 능력, 초자연적인 이동 속도와 재생능력, 그리고 더 많은 무리원들이 합류함에 따라 더욱 강해지는 전투의 포효 능력을 가지고 있습니다.\n\n라이칸의 역사에 대해 확립된 명확한 역사는 없으며, 특히 그들의 무리는 자신의 기원을 조작하는 경향이 있기 때문에 더욱 모호합니다. 이것은 매우 다양한 음모론으로 이어졌으며, 특히 유전자의 유사성 때문에 많은 사람들이 부분적으로라도 생귀오파지와 관련이 있다고 생각합니다. 가장 일반적인 가설은 생귀오파지가 이타킨과 사랑에 빠졌고, 나중에 그들의 아이가 변이되었다는 것이지만, 또 다른 이야기에선 생귀오파지가 임신한 후 여러 복잡한 문제가 덮쳐왔고. 아이는 태어났지만 부모에게 버림받았으며 길 잃은 개들 사이에서 길러졌다는 것 입니다. 결국 그들은 혈육보다 끈끈한 유대로 자신의 가족을 만들었고, 가족이 최우선 이라는 것을 항상 마음에 새겼다는 것입니다.</t>
+  </si>
+  <si>
+    <t>울프맨/라이칸은 기원이 불분명한 인종형으로, 영토를 확장하며 무리 또는 더 큰 씨족을 형성하기 위해 변방계 곳곳에 전파되었습니다. 그들의 울프맨 형태는 야행성 능력을 감소시키고, 그들의 유전자를 다른 사람들과 공유할 수 있는 대가로 많은 이점을 포기했습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>울프맨/라이칸은 기원이 불분명한 인종형으로, 영토를 확장하며 무리 또는 더 큰 씨족을 형성하기 위해 변방계 곳곳에 전파되었습니다. 그들의 라이칸 형태는 야행성의 이점, 향상된 근접 전투 능력, 초자연적인 이동 속도와 재생능력, 그리고 더 많은 무리원들이 합류함에 따라 더욱 강해지는 전투의 포효 능력을 가지고 있습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TargetA의 생식유전자 추출하는 중</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pack mentality</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기본적으로, 빛 공포증을 가진 폰이 빛으로부터 달아날 때마다 게임은 플레이어에게 이를 알리는 편지를 생성합니다. 많은 폰이 자주 도망친다면 이것은 다소 짜증나며 게임 플레이에 영향이 있을 수 있으므로, 이 옵션으로 비활성화할 수 있습니다. 폰들이 여전히 도망친다는 것을 명심하십시오. 메세지를 받지 못할 뿐입니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>빛 공포증</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>경고: {PAWN_nameDef}의 유전자가 재성장중 입니다. {PAWN_possessive} 유전자가 완전히 재성장 되기 전에 변형이식체를 심게 되면 {PAWN_pronoun}(은)는 죽습니다.\n\n계속하시겠습니까?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>여기는 빛이 너무 많아. 눈이 아프다고!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>우리 무리원이 죽었어. 무리가 약해질거야.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>소중한 무리원 중 한 명을 잃었어. 그들이 무리가 없이 살아남을 수 있을까?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>무리 동료 {0} 버려짐</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>무리 동료 {0} 팔아넘김</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이 사람은 매우 빠르게 움직입니다. 이동 시 지형에 따른 불이익을 무시합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전투의 포효로 인해 능력이 향상되었습니다. 최대 10회 중첩되며, 3시간 동안 지속됩니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이 유전자의 보유자는 대화를 이해하고 말하는 능력을 잃습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이 유전자의 보유자는 늑대처럼 생긴 꼬리가 자라나며, 움직이는데 약간 도움이 됩니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이 유전자를 보유한 남성은 얼굴 측면에 엄청난 속도로 수염이 자랍니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이 유전자의 보유자는 빛이 잘 드는 지역보다 어둠 속을 훨씬 더 잘 볼 수 있으며, 어둠과 관련된 기분 불이익에 영향을 받지 않습니다. 망막 뒤에 어둠 속에서 보는 능력을 증폭시키는 반사층을 가지고 있습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이 유전자의 보유자는 아군의 사기를 드높이는 강렬한 포효를 사용할 수 있으며, 아군의 공세를 더욱 거세게 만들 수 있습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이 유전자의 보유자는 눈에 생물학적 화합물을 가지고 있는데, 이 화합물은 빛의 광자에 고통스럽게 반응합니다. 어떤 광원에도 매우 민감합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이 유전자의 보유자는 눈에 빛 광자에 위험하게 반응하는 생물학적 화합물을 가지고 있습니다. 어떤 광원에도 비정상적으로 민감합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이 유전자의 보유자는 공격을 매우 쉽게 피할 수 있습니다. 인지 능력이 뛰어나기 때문에 공격이 본능적으로 피해집니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이 유전자의 보유자는 공격을 피할 수 없습니다. 전투 인지 능력이 부족해 모든 공격이 적중당하며, 심지어 빗나갈 공격에도 맞습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이 유전자의 보유자는 밤에 일하는 것을 선호합니다. 밤에 깨어 있으면 더 행복해지고, 낮에 깨어 있으면 불행해집니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>letterTextBeggarsBetrayed-&gt;울프맨 난민들은 당신에게 배신당했으며, 자신들을 최대한 보호하려고 할 것입니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Merge_galler0 [Not chosen]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2933,10 +3429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F173"/>
+  <dimension ref="A1:G173"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -2947,9 +3443,10 @@
     <col min="4" max="4" width="41.1640625" customWidth="1"/>
     <col min="5" max="5" width="46" customWidth="1"/>
     <col min="6" max="6" width="47.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="44" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2968,8 +3465,11 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G1" s="2" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -2988,8 +3488,11 @@
       <c r="F2" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G2" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
@@ -3008,8 +3511,11 @@
       <c r="F3" s="4" t="s">
         <v>542</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G3" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -3028,8 +3534,11 @@
       <c r="F4" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G4" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="5" t="s">
         <v>18</v>
       </c>
@@ -3040,16 +3549,19 @@
         <v>19</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>541</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G5" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -3065,8 +3577,11 @@
       <c r="E6" s="9" t="s">
         <v>518</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G6" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="5" t="s">
         <v>23</v>
       </c>
@@ -3077,16 +3592,19 @@
         <v>24</v>
       </c>
       <c r="D7" s="5" t="s">
+        <v>632</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>635</v>
+      </c>
+      <c r="F7" s="11" t="s">
         <v>634</v>
       </c>
-      <c r="E7" s="14" t="s">
-        <v>637</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>636</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G7" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
@@ -3102,8 +3620,11 @@
       <c r="E8" s="9" t="s">
         <v>553</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G8" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>29</v>
       </c>
@@ -3119,8 +3640,11 @@
       <c r="E9" s="9" t="s">
         <v>566</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G9" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>33</v>
       </c>
@@ -3136,8 +3660,11 @@
       <c r="E10" s="9" t="s">
         <v>568</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G10" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>35</v>
       </c>
@@ -3153,8 +3680,11 @@
       <c r="E11" s="9" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G11" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>38</v>
       </c>
@@ -3170,8 +3700,11 @@
       <c r="E12" s="9" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G12" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>41</v>
       </c>
@@ -3187,8 +3720,11 @@
       <c r="E13" s="9" t="s">
         <v>571</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G13" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>44</v>
       </c>
@@ -3204,8 +3740,11 @@
       <c r="E14" s="9" t="s">
         <v>572</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G14" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>47</v>
       </c>
@@ -3221,8 +3760,11 @@
       <c r="E15" s="9" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G15" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>50</v>
       </c>
@@ -3238,8 +3780,11 @@
       <c r="E16" s="9" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G16" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>52</v>
       </c>
@@ -3255,8 +3800,11 @@
       <c r="E17" s="9" t="s">
         <v>576</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G17" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>55</v>
       </c>
@@ -3272,8 +3820,11 @@
       <c r="E18" s="9" t="s">
         <v>577</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G18" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="5" t="s">
         <v>58</v>
       </c>
@@ -3289,8 +3840,11 @@
       <c r="E19" s="10" t="s">
         <v>578</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G19" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>61</v>
       </c>
@@ -3303,9 +3857,14 @@
       <c r="D20" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="E20" s="7" t="s">
+        <v>656</v>
+      </c>
+      <c r="G20" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>65</v>
       </c>
@@ -3318,9 +3877,14 @@
       <c r="D21" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="E21" s="7" t="s">
+        <v>656</v>
+      </c>
+      <c r="G21" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>67</v>
       </c>
@@ -3333,9 +3897,14 @@
       <c r="D22" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E22" s="1"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="E22" s="7" t="s">
+        <v>656</v>
+      </c>
+      <c r="G22" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>69</v>
       </c>
@@ -3351,8 +3920,11 @@
       <c r="E23" s="7" t="s">
         <v>545</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G23" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="5" t="s">
         <v>72</v>
       </c>
@@ -3368,8 +3940,11 @@
       <c r="E24" s="8" t="s">
         <v>544</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G24" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>75</v>
       </c>
@@ -3385,8 +3960,11 @@
       <c r="E25" s="9" t="s">
         <v>546</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G25" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="5" t="s">
         <v>79</v>
       </c>
@@ -3402,8 +3980,11 @@
       <c r="E26" s="10" t="s">
         <v>547</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G26" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>82</v>
       </c>
@@ -3419,8 +4000,11 @@
       <c r="E27" s="9" t="s">
         <v>533</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G27" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>85</v>
       </c>
@@ -3431,11 +4015,16 @@
         <v>19</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>635</v>
-      </c>
-      <c r="E28" s="1"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+        <v>633</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>782</v>
+      </c>
+      <c r="G28" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="5" t="s">
         <v>86</v>
       </c>
@@ -3449,10 +4038,13 @@
         <v>88</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>612</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+        <v>610</v>
+      </c>
+      <c r="G29" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
         <v>89</v>
       </c>
@@ -3468,8 +4060,11 @@
       <c r="E30" s="9" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G30" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
         <v>92</v>
       </c>
@@ -3485,8 +4080,11 @@
       <c r="E31" s="9" t="s">
         <v>540</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G31" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" s="5" t="s">
         <v>95</v>
       </c>
@@ -3505,8 +4103,11 @@
       <c r="F32" s="11" t="s">
         <v>592</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G32" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
         <v>98</v>
       </c>
@@ -3522,8 +4123,11 @@
       <c r="E33" s="9" t="s">
         <v>538</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G33" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34" s="5" t="s">
         <v>101</v>
       </c>
@@ -3536,9 +4140,14 @@
       <c r="D34" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="E34" s="5"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E34" s="10" t="s">
+        <v>665</v>
+      </c>
+      <c r="G34" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
         <v>104</v>
       </c>
@@ -3554,8 +4163,11 @@
       <c r="E35" s="9" t="s">
         <v>534</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G35" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" s="5" t="s">
         <v>107</v>
       </c>
@@ -3568,9 +4180,14 @@
       <c r="D36" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="E36" s="5"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E36" s="10" t="s">
+        <v>778</v>
+      </c>
+      <c r="G36" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
         <v>110</v>
       </c>
@@ -3586,8 +4203,11 @@
       <c r="E37" s="9" t="s">
         <v>549</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G37" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A38" s="5" t="s">
         <v>113</v>
       </c>
@@ -3600,9 +4220,14 @@
       <c r="D38" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="E38" s="5"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E38" s="10" t="s">
+        <v>669</v>
+      </c>
+      <c r="G38" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
         <v>116</v>
       </c>
@@ -3618,8 +4243,11 @@
       <c r="E39" s="9" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G39" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A40" s="5" t="s">
         <v>119</v>
       </c>
@@ -3632,9 +4260,14 @@
       <c r="D40" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="E40" s="5"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E40" s="10" t="s">
+        <v>671</v>
+      </c>
+      <c r="G40" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
         <v>122</v>
       </c>
@@ -3650,8 +4283,11 @@
       <c r="E41" s="9" t="s">
         <v>535</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G41" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A42" s="5" t="s">
         <v>125</v>
       </c>
@@ -3664,9 +4300,14 @@
       <c r="D42" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="E42" s="5"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E42" s="10" t="s">
+        <v>779</v>
+      </c>
+      <c r="G42" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
         <v>128</v>
       </c>
@@ -3682,8 +4323,11 @@
       <c r="E43" s="9" t="s">
         <v>537</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G43" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A44" s="5" t="s">
         <v>130</v>
       </c>
@@ -3696,9 +4340,14 @@
       <c r="D44" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="E44" s="5"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E44" s="10" t="s">
+        <v>780</v>
+      </c>
+      <c r="G44" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
         <v>133</v>
       </c>
@@ -3714,8 +4363,11 @@
       <c r="E45" s="9" t="s">
         <v>591</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G45" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
         <v>136</v>
       </c>
@@ -3728,9 +4380,14 @@
       <c r="D46" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="E46" s="1"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E46" s="7" t="s">
+        <v>781</v>
+      </c>
+      <c r="G46" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
         <v>139</v>
       </c>
@@ -3744,8 +4401,11 @@
         <v>141</v>
       </c>
       <c r="E47" s="1"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G47" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
         <v>142</v>
       </c>
@@ -3759,8 +4419,11 @@
         <v>144</v>
       </c>
       <c r="E48" s="1"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G48" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
         <v>145</v>
       </c>
@@ -3774,8 +4437,11 @@
         <v>147</v>
       </c>
       <c r="E49" s="1"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G49" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
         <v>148</v>
       </c>
@@ -3789,8 +4455,11 @@
         <v>150</v>
       </c>
       <c r="E50" s="1"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G50" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
         <v>151</v>
       </c>
@@ -3804,8 +4473,11 @@
         <v>153</v>
       </c>
       <c r="E51" s="1"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G51" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
         <v>154</v>
       </c>
@@ -3819,8 +4491,11 @@
         <v>156</v>
       </c>
       <c r="E52" s="1"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G52" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A53" s="1" t="s">
         <v>157</v>
       </c>
@@ -3834,8 +4509,11 @@
         <v>159</v>
       </c>
       <c r="E53" s="1"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G53" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A54" s="5" t="s">
         <v>160</v>
       </c>
@@ -3849,8 +4527,11 @@
         <v>162</v>
       </c>
       <c r="E54" s="5"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G54" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
         <v>163</v>
       </c>
@@ -3866,8 +4547,11 @@
       <c r="E55" s="9" t="s">
         <v>551</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G55" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A56" s="5" t="s">
         <v>166</v>
       </c>
@@ -3880,9 +4564,14 @@
       <c r="D56" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="E56" s="5"/>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E56" s="8" t="s">
+        <v>783</v>
+      </c>
+      <c r="G56" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A57" s="1" t="s">
         <v>169</v>
       </c>
@@ -3898,8 +4587,11 @@
       <c r="E57" s="9" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G57" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A58" s="5" t="s">
         <v>172</v>
       </c>
@@ -3912,9 +4604,14 @@
       <c r="D58" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="E58" s="5"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E58" s="8" t="s">
+        <v>784</v>
+      </c>
+      <c r="G58" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A59" s="1" t="s">
         <v>175</v>
       </c>
@@ -3930,8 +4627,11 @@
       <c r="E59" s="9" t="s">
         <v>554</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G59" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A60" s="5" t="s">
         <v>178</v>
       </c>
@@ -3944,9 +4644,14 @@
       <c r="D60" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="E60" s="5"/>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E60" s="8" t="s">
+        <v>683</v>
+      </c>
+      <c r="G60" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A61" s="1" t="s">
         <v>181</v>
       </c>
@@ -3962,8 +4667,11 @@
       <c r="E61" s="9" t="s">
         <v>555</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G61" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A62" s="5" t="s">
         <v>184</v>
       </c>
@@ -3976,9 +4684,14 @@
       <c r="D62" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="E62" s="5"/>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E62" s="8" t="s">
+        <v>785</v>
+      </c>
+      <c r="G62" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A63" s="1" t="s">
         <v>187</v>
       </c>
@@ -3994,8 +4707,11 @@
       <c r="E63" s="9" t="s">
         <v>556</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G63" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A64" s="5" t="s">
         <v>190</v>
       </c>
@@ -4008,9 +4724,14 @@
       <c r="D64" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="E64" s="5"/>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E64" s="8" t="s">
+        <v>786</v>
+      </c>
+      <c r="G64" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A65" s="1" t="s">
         <v>193</v>
       </c>
@@ -4026,8 +4747,11 @@
       <c r="E65" s="9" t="s">
         <v>550</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G65" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A66" s="5" t="s">
         <v>196</v>
       </c>
@@ -4040,9 +4764,14 @@
       <c r="D66" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="E66" s="5"/>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E66" s="8" t="s">
+        <v>689</v>
+      </c>
+      <c r="G66" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A67" s="1" t="s">
         <v>199</v>
       </c>
@@ -4058,8 +4787,11 @@
       <c r="E67" s="9" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G67" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A68" s="5" t="s">
         <v>202</v>
       </c>
@@ -4075,8 +4807,11 @@
       <c r="E68" s="8" t="s">
         <v>595</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G68" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A69" s="1" t="s">
         <v>204</v>
       </c>
@@ -4092,8 +4827,11 @@
       <c r="E69" s="9" t="s">
         <v>516</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G69" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A70" s="5" t="s">
         <v>207</v>
       </c>
@@ -4109,8 +4847,11 @@
       <c r="E70" s="8" t="s">
         <v>597</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G70" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A71" s="1" t="s">
         <v>209</v>
       </c>
@@ -4124,10 +4865,13 @@
         <v>211</v>
       </c>
       <c r="E71" s="9" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.45">
+        <v>605</v>
+      </c>
+      <c r="G71" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A72" s="5" t="s">
         <v>212</v>
       </c>
@@ -4141,10 +4885,13 @@
         <v>214</v>
       </c>
       <c r="E72" s="8" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.45">
+        <v>631</v>
+      </c>
+      <c r="G72" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A73" s="1" t="s">
         <v>215</v>
       </c>
@@ -4158,10 +4905,13 @@
         <v>217</v>
       </c>
       <c r="E73" s="9" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.45">
+        <v>606</v>
+      </c>
+      <c r="G73" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A74" s="5" t="s">
         <v>218</v>
       </c>
@@ -4177,8 +4927,11 @@
       <c r="E74" s="8" t="s">
         <v>598</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G74" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A75" s="1" t="s">
         <v>221</v>
       </c>
@@ -4192,10 +4945,13 @@
         <v>223</v>
       </c>
       <c r="E75" s="9" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.45">
+        <v>607</v>
+      </c>
+      <c r="G75" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A76" s="5" t="s">
         <v>224</v>
       </c>
@@ -4211,8 +4967,11 @@
       <c r="E76" s="8" t="s">
         <v>599</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G76" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A77" s="1" t="s">
         <v>227</v>
       </c>
@@ -4226,10 +4985,13 @@
         <v>229</v>
       </c>
       <c r="E77" s="9" t="s">
-        <v>610</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.45">
+        <v>608</v>
+      </c>
+      <c r="G77" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A78" s="5" t="s">
         <v>230</v>
       </c>
@@ -4245,8 +5007,11 @@
       <c r="E78" s="8" t="s">
         <v>600</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G78" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A79" s="1" t="s">
         <v>233</v>
       </c>
@@ -4260,10 +5025,13 @@
         <v>235</v>
       </c>
       <c r="E79" s="9" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.45">
+        <v>609</v>
+      </c>
+      <c r="G79" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A80" s="5" t="s">
         <v>236</v>
       </c>
@@ -4279,8 +5047,11 @@
       <c r="E80" s="8" t="s">
         <v>601</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G80" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A81" s="1" t="s">
         <v>239</v>
       </c>
@@ -4296,8 +5067,11 @@
       <c r="E81" s="9" t="s">
         <v>515</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G81" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A82" s="5" t="s">
         <v>242</v>
       </c>
@@ -4310,9 +5084,14 @@
       <c r="D82" s="5" t="s">
         <v>244</v>
       </c>
-      <c r="E82" s="5"/>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="E82" s="8" t="s">
+        <v>787</v>
+      </c>
+      <c r="G82" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A83" s="1" t="s">
         <v>245</v>
       </c>
@@ -4331,8 +5110,11 @@
       <c r="F83" s="11" t="s">
         <v>558</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G83" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A84" s="1" t="s">
         <v>248</v>
       </c>
@@ -4346,8 +5128,11 @@
         <v>250</v>
       </c>
       <c r="E84" s="1"/>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G84" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A85" s="1" t="s">
         <v>251</v>
       </c>
@@ -4363,8 +5148,11 @@
       <c r="E85" s="9" t="s">
         <v>560</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G85" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A86" s="1" t="s">
         <v>254</v>
       </c>
@@ -4380,8 +5168,11 @@
       <c r="E86" s="9" t="s">
         <v>559</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G86" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A87" s="1" t="s">
         <v>257</v>
       </c>
@@ -4395,8 +5186,11 @@
         <v>259</v>
       </c>
       <c r="E87" s="1"/>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G87" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A88" s="1" t="s">
         <v>260</v>
       </c>
@@ -4410,8 +5204,11 @@
         <v>262</v>
       </c>
       <c r="E88" s="1"/>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G88" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A89" s="1" t="s">
         <v>263</v>
       </c>
@@ -4425,8 +5222,11 @@
         <v>265</v>
       </c>
       <c r="E89" s="1"/>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G89" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A90" s="1" t="s">
         <v>266</v>
       </c>
@@ -4440,8 +5240,11 @@
         <v>268</v>
       </c>
       <c r="E90" s="1"/>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G90" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A91" s="1" t="s">
         <v>269</v>
       </c>
@@ -4455,8 +5258,11 @@
         <v>271</v>
       </c>
       <c r="E91" s="1"/>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G91" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A92" s="1" t="s">
         <v>272</v>
       </c>
@@ -4470,8 +5276,11 @@
         <v>274</v>
       </c>
       <c r="E92" s="1"/>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G92" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A93" s="1" t="s">
         <v>275</v>
       </c>
@@ -4485,8 +5294,11 @@
         <v>277</v>
       </c>
       <c r="E93" s="1"/>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G93" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A94" s="1" t="s">
         <v>278</v>
       </c>
@@ -4500,8 +5312,11 @@
         <v>280</v>
       </c>
       <c r="E94" s="1"/>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G94" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A95" s="1" t="s">
         <v>281</v>
       </c>
@@ -4515,8 +5330,11 @@
         <v>280</v>
       </c>
       <c r="E95" s="1"/>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G95" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A96" s="1" t="s">
         <v>283</v>
       </c>
@@ -4530,8 +5348,11 @@
         <v>285</v>
       </c>
       <c r="E96" s="1"/>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G96" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A97" s="5" t="s">
         <v>286</v>
       </c>
@@ -4545,8 +5366,11 @@
         <v>288</v>
       </c>
       <c r="E97" s="5"/>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G97" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A98" s="1" t="s">
         <v>289</v>
       </c>
@@ -4562,8 +5386,11 @@
       <c r="E98" s="9" t="s">
         <v>543</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G98" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A99" s="5" t="s">
         <v>292</v>
       </c>
@@ -4574,13 +5401,16 @@
         <v>293</v>
       </c>
       <c r="D99" s="5" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="E99" s="10" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.45">
+        <v>619</v>
+      </c>
+      <c r="G99" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A100" s="1" t="s">
         <v>294</v>
       </c>
@@ -4596,8 +5426,11 @@
       <c r="E100" s="9" t="s">
         <v>511</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G100" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A101" s="1" t="s">
         <v>297</v>
       </c>
@@ -4610,9 +5443,14 @@
       <c r="D101" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="E101" s="1"/>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E101" s="7" t="s">
+        <v>761</v>
+      </c>
+      <c r="G101" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A102" s="5" t="s">
         <v>300</v>
       </c>
@@ -4625,9 +5463,14 @@
       <c r="D102" s="5" t="s">
         <v>302</v>
       </c>
-      <c r="E102" s="5"/>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E102" s="8" t="s">
+        <v>764</v>
+      </c>
+      <c r="G102" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A103" s="1" t="s">
         <v>303</v>
       </c>
@@ -4643,8 +5486,11 @@
       <c r="E103" s="9" t="s">
         <v>512</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G103" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A104" s="1" t="s">
         <v>306</v>
       </c>
@@ -4657,9 +5503,14 @@
       <c r="D104" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="E104" s="1"/>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E104" s="7" t="s">
+        <v>763</v>
+      </c>
+      <c r="G104" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A105" s="5" t="s">
         <v>309</v>
       </c>
@@ -4672,9 +5523,14 @@
       <c r="D105" s="5" t="s">
         <v>311</v>
       </c>
-      <c r="E105" s="5"/>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E105" s="8" t="s">
+        <v>765</v>
+      </c>
+      <c r="G105" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A106" s="1" t="s">
         <v>312</v>
       </c>
@@ -4690,8 +5546,11 @@
       <c r="E106" s="9" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G106" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A107" s="1" t="s">
         <v>315</v>
       </c>
@@ -4704,9 +5563,14 @@
       <c r="D107" s="5" t="s">
         <v>316</v>
       </c>
-      <c r="E107" s="5"/>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E107" s="8" t="s">
+        <v>776</v>
+      </c>
+      <c r="G107" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A108" s="1" t="s">
         <v>317</v>
       </c>
@@ -4722,8 +5586,11 @@
       <c r="E108" s="9" t="s">
         <v>533</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G108" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A109" s="1" t="s">
         <v>319</v>
       </c>
@@ -4736,9 +5603,14 @@
       <c r="D109" s="5" t="s">
         <v>321</v>
       </c>
-      <c r="E109" s="5"/>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E109" s="8" t="s">
+        <v>777</v>
+      </c>
+      <c r="G109" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A110" s="1" t="s">
         <v>322</v>
       </c>
@@ -4754,8 +5626,11 @@
       <c r="E110" s="7" t="s">
         <v>603</v>
       </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G110" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A111" s="1" t="s">
         <v>325</v>
       </c>
@@ -4768,9 +5643,14 @@
       <c r="D111" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="E111" s="1"/>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E111" s="7" t="s">
+        <v>713</v>
+      </c>
+      <c r="G111" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A112" s="1" t="s">
         <v>328</v>
       </c>
@@ -4786,8 +5666,11 @@
       <c r="E112" s="7" t="s">
         <v>602</v>
       </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G112" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A113" s="5" t="s">
         <v>331</v>
       </c>
@@ -4800,9 +5683,14 @@
       <c r="D113" s="5" t="s">
         <v>333</v>
       </c>
-      <c r="E113" s="5"/>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="E113" s="8" t="s">
+        <v>715</v>
+      </c>
+      <c r="G113" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A114" s="5" t="s">
         <v>334</v>
       </c>
@@ -4815,9 +5703,14 @@
       <c r="D114" s="5" t="s">
         <v>337</v>
       </c>
-      <c r="E114" s="5"/>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="E114" s="8" t="s">
+        <v>766</v>
+      </c>
+      <c r="G114" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A115" s="1" t="s">
         <v>338</v>
       </c>
@@ -4830,12 +5723,17 @@
       <c r="D115" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="E115" s="1"/>
+      <c r="E115" s="7" t="s">
+        <v>769</v>
+      </c>
       <c r="F115" s="12" t="s">
         <v>581</v>
       </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G115" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A116" s="1" t="s">
         <v>341</v>
       </c>
@@ -4854,8 +5752,11 @@
       <c r="F116" s="12" t="s">
         <v>580</v>
       </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G116" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A117" s="1" t="s">
         <v>344</v>
       </c>
@@ -4874,8 +5775,11 @@
       <c r="F117" s="12" t="s">
         <v>565</v>
       </c>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G117" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A118" s="1" t="s">
         <v>347</v>
       </c>
@@ -4894,8 +5798,11 @@
       <c r="F118" s="12" t="s">
         <v>563</v>
       </c>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G118" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A119" s="1" t="s">
         <v>350</v>
       </c>
@@ -4914,8 +5821,11 @@
       <c r="F119" s="12" t="s">
         <v>564</v>
       </c>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G119" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A120" s="5" t="s">
         <v>353</v>
       </c>
@@ -4934,8 +5844,11 @@
       <c r="F120" s="12" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G120" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A121" s="5" t="s">
         <v>356</v>
       </c>
@@ -4949,10 +5862,13 @@
         <v>64</v>
       </c>
       <c r="E121" s="10" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.45">
+        <v>615</v>
+      </c>
+      <c r="G121" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A122" s="1" t="s">
         <v>359</v>
       </c>
@@ -4968,8 +5884,11 @@
       <c r="E122" s="7" t="s">
         <v>586</v>
       </c>
-    </row>
-    <row r="123" spans="1:6" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="G122" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A123" s="5" t="s">
         <v>363</v>
       </c>
@@ -4985,8 +5904,11 @@
       <c r="E123" s="8" t="s">
         <v>586</v>
       </c>
-    </row>
-    <row r="124" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="G123" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A124" s="1" t="s">
         <v>365</v>
       </c>
@@ -5000,8 +5922,11 @@
         <v>368</v>
       </c>
       <c r="E124" s="6"/>
-    </row>
-    <row r="125" spans="1:6" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="G124" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A125" s="1" t="s">
         <v>369</v>
       </c>
@@ -5017,8 +5942,11 @@
       <c r="E125" s="9" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G125" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A126" s="1" t="s">
         <v>372</v>
       </c>
@@ -5034,8 +5962,11 @@
       <c r="E126" s="9" t="s">
         <v>525</v>
       </c>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G126" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A127" s="1" t="s">
         <v>375</v>
       </c>
@@ -5051,8 +5982,11 @@
       <c r="E127" s="9" t="s">
         <v>520</v>
       </c>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G127" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A128" s="1" t="s">
         <v>378</v>
       </c>
@@ -5068,8 +6002,11 @@
       <c r="E128" s="9" t="s">
         <v>521</v>
       </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G128" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A129" s="1" t="s">
         <v>381</v>
       </c>
@@ -5085,8 +6022,11 @@
       <c r="E129" s="9" t="s">
         <v>522</v>
       </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G129" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A130" s="1" t="s">
         <v>384</v>
       </c>
@@ -5102,8 +6042,11 @@
       <c r="E130" s="9" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G130" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A131" s="1" t="s">
         <v>387</v>
       </c>
@@ -5119,8 +6062,11 @@
       <c r="E131" s="9" t="s">
         <v>524</v>
       </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G131" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A132" s="1" t="s">
         <v>390</v>
       </c>
@@ -5136,8 +6082,11 @@
       <c r="E132" s="9" t="s">
         <v>527</v>
       </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G132" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A133" s="1" t="s">
         <v>393</v>
       </c>
@@ -5153,8 +6102,11 @@
       <c r="E133" s="9" t="s">
         <v>526</v>
       </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G133" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A134" s="1" t="s">
         <v>396</v>
       </c>
@@ -5170,8 +6122,11 @@
       <c r="E134" s="9" t="s">
         <v>528</v>
       </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G134" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A135" s="1" t="s">
         <v>399</v>
       </c>
@@ -5187,8 +6142,11 @@
       <c r="E135" s="9" t="s">
         <v>529</v>
       </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G135" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A136" s="1" t="s">
         <v>402</v>
       </c>
@@ -5204,8 +6162,11 @@
       <c r="E136" s="9" t="s">
         <v>530</v>
       </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G136" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A137" s="1" t="s">
         <v>405</v>
       </c>
@@ -5221,8 +6182,11 @@
       <c r="E137" s="9" t="s">
         <v>531</v>
       </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G137" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A138" s="1" t="s">
         <v>408</v>
       </c>
@@ -5238,8 +6202,11 @@
       <c r="E138" s="9" t="s">
         <v>532</v>
       </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G138" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A139" s="1" t="s">
         <v>411</v>
       </c>
@@ -5250,13 +6217,16 @@
         <v>412</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="E139" s="9" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.45">
+        <v>623</v>
+      </c>
+      <c r="G139" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A140" s="1" t="s">
         <v>413</v>
       </c>
@@ -5269,9 +6239,14 @@
       <c r="D140" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="E140" s="1"/>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E140" s="7" t="s">
+        <v>739</v>
+      </c>
+      <c r="G140" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A141" s="1" t="s">
         <v>416</v>
       </c>
@@ -5285,10 +6260,13 @@
         <v>418</v>
       </c>
       <c r="E141" s="9" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.45">
+        <v>624</v>
+      </c>
+      <c r="G141" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A142" s="1" t="s">
         <v>419</v>
       </c>
@@ -5299,13 +6277,16 @@
         <v>420</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="E142" s="7" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.45">
+        <v>629</v>
+      </c>
+      <c r="G142" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A143" s="1" t="s">
         <v>421</v>
       </c>
@@ -5319,10 +6300,13 @@
         <v>423</v>
       </c>
       <c r="E143" s="9" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.45">
+        <v>625</v>
+      </c>
+      <c r="G143" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A144" s="1" t="s">
         <v>424</v>
       </c>
@@ -5336,10 +6320,13 @@
         <v>426</v>
       </c>
       <c r="E144" s="7" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.45">
+        <v>626</v>
+      </c>
+      <c r="G144" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A145" s="1" t="s">
         <v>427</v>
       </c>
@@ -5353,10 +6340,13 @@
         <v>429</v>
       </c>
       <c r="E145" s="7" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.45">
+        <v>627</v>
+      </c>
+      <c r="G145" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A146" s="5" t="s">
         <v>430</v>
       </c>
@@ -5367,11 +6357,16 @@
         <v>431</v>
       </c>
       <c r="D146" s="5" t="s">
-        <v>632</v>
-      </c>
-      <c r="E146" s="5"/>
-    </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.45">
+        <v>630</v>
+      </c>
+      <c r="E146" s="8" t="s">
+        <v>788</v>
+      </c>
+      <c r="G146" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A147" s="1" t="s">
         <v>432</v>
       </c>
@@ -5390,8 +6385,11 @@
       <c r="F147" s="11" t="s">
         <v>588</v>
       </c>
-    </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G147" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A148" s="1" t="s">
         <v>435</v>
       </c>
@@ -5404,9 +6402,14 @@
       <c r="D148" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="E148" s="1"/>
-    </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="E148" s="7" t="s">
+        <v>746</v>
+      </c>
+      <c r="G148" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A149" s="1" t="s">
         <v>438</v>
       </c>
@@ -5422,8 +6425,11 @@
       <c r="E149" s="9" t="s">
         <v>587</v>
       </c>
-    </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G149" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A150" s="1" t="s">
         <v>440</v>
       </c>
@@ -5436,9 +6442,14 @@
       <c r="D150" s="1" t="s">
         <v>442</v>
       </c>
-      <c r="E150" s="1"/>
-    </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="E150" s="7" t="s">
+        <v>771</v>
+      </c>
+      <c r="G150" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A151" s="1" t="s">
         <v>443</v>
       </c>
@@ -5454,8 +6465,11 @@
       <c r="E151" s="9" t="s">
         <v>550</v>
       </c>
-    </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G151" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A152" s="1" t="s">
         <v>446</v>
       </c>
@@ -5468,9 +6482,14 @@
       <c r="D152" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="E152" s="1"/>
-    </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="E152" s="7" t="s">
+        <v>749</v>
+      </c>
+      <c r="G152" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A153" s="1" t="s">
         <v>449</v>
       </c>
@@ -5486,8 +6505,11 @@
       <c r="E153" s="7" t="s">
         <v>604</v>
       </c>
-    </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G153" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A154" s="1" t="s">
         <v>452</v>
       </c>
@@ -5500,9 +6522,14 @@
       <c r="D154" s="1" t="s">
         <v>454</v>
       </c>
-      <c r="E154" s="1"/>
-    </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="E154" s="7" t="s">
+        <v>772</v>
+      </c>
+      <c r="G154" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A155" s="1" t="s">
         <v>455</v>
       </c>
@@ -5516,10 +6543,13 @@
         <v>457</v>
       </c>
       <c r="E155" s="7" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="156" spans="1:6" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+        <v>774</v>
+      </c>
+      <c r="G155" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A156" s="1" t="s">
         <v>458</v>
       </c>
@@ -5532,9 +6562,14 @@
       <c r="D156" s="1" t="s">
         <v>460</v>
       </c>
-      <c r="E156" s="1"/>
-    </row>
-    <row r="157" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="E156" s="7" t="s">
+        <v>773</v>
+      </c>
+      <c r="G156" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A157" s="1" t="s">
         <v>461</v>
       </c>
@@ -5548,8 +6583,11 @@
         <v>463</v>
       </c>
       <c r="E157" s="6"/>
-    </row>
-    <row r="158" spans="1:6" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="G157" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A158" s="1" t="s">
         <v>464</v>
       </c>
@@ -5563,10 +6601,13 @@
         <v>466</v>
       </c>
       <c r="E158" s="7" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.45">
+        <v>775</v>
+      </c>
+      <c r="G158" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A159" s="1" t="s">
         <v>467</v>
       </c>
@@ -5579,9 +6620,14 @@
       <c r="D159" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="E159" s="1"/>
-    </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="E159" s="7" t="s">
+        <v>756</v>
+      </c>
+      <c r="G159" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A160" s="1" t="s">
         <v>470</v>
       </c>
@@ -5594,9 +6640,14 @@
       <c r="D160" s="1" t="s">
         <v>472</v>
       </c>
-      <c r="E160" s="1"/>
-    </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="E160" s="7" t="s">
+        <v>757</v>
+      </c>
+      <c r="G160" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A161" s="1" t="s">
         <v>473</v>
       </c>
@@ -5607,13 +6658,16 @@
         <v>474</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>201</v>
+        <v>767</v>
       </c>
       <c r="E161" s="7" t="s">
         <v>590</v>
       </c>
-    </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G161" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A162" s="5" t="s">
         <v>475</v>
       </c>
@@ -5626,9 +6680,14 @@
       <c r="D162" s="5" t="s">
         <v>477</v>
       </c>
-      <c r="E162" s="5"/>
-    </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="E162" s="8" t="s">
+        <v>758</v>
+      </c>
+      <c r="G162" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A163" s="1" t="s">
         <v>478</v>
       </c>
@@ -5644,8 +6703,11 @@
       <c r="E163" s="9" t="s">
         <v>589</v>
       </c>
-    </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G163" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A164" s="5" t="s">
         <v>482</v>
       </c>
@@ -5658,9 +6720,14 @@
       <c r="D164" s="5" t="s">
         <v>484</v>
       </c>
-      <c r="E164" s="5"/>
-    </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="E164" s="8" t="s">
+        <v>768</v>
+      </c>
+      <c r="G164" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A165" s="1" t="s">
         <v>485</v>
       </c>
@@ -5674,10 +6741,13 @@
         <v>487</v>
       </c>
       <c r="E165" s="7" t="s">
-        <v>615</v>
-      </c>
-    </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.45">
+        <v>613</v>
+      </c>
+      <c r="G165" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A166" s="1" t="s">
         <v>488</v>
       </c>
@@ -5688,13 +6758,16 @@
         <v>489</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="E166" s="7" t="s">
-        <v>614</v>
-      </c>
-    </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.45">
+        <v>612</v>
+      </c>
+      <c r="G166" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A167" s="1" t="s">
         <v>490</v>
       </c>
@@ -5707,12 +6780,17 @@
       <c r="D167" s="1" t="s">
         <v>492</v>
       </c>
-      <c r="E167" s="1"/>
+      <c r="E167" s="7" t="s">
+        <v>770</v>
+      </c>
       <c r="F167" s="1" t="s">
-        <v>616</v>
-      </c>
-    </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.45">
+        <v>614</v>
+      </c>
+      <c r="G167" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A168" s="1" t="s">
         <v>493</v>
       </c>
@@ -5726,8 +6804,11 @@
         <v>495</v>
       </c>
       <c r="E168" s="1"/>
-    </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G168" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A169" s="1" t="s">
         <v>496</v>
       </c>
@@ -5741,8 +6822,11 @@
         <v>498</v>
       </c>
       <c r="E169" s="1"/>
-    </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G169" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A170" s="1" t="s">
         <v>499</v>
       </c>
@@ -5756,8 +6840,11 @@
         <v>501</v>
       </c>
       <c r="E170" s="1"/>
-    </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G170" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A171" s="1" t="s">
         <v>502</v>
       </c>
@@ -5771,13 +6858,16 @@
         <v>504</v>
       </c>
       <c r="E171" s="7" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="F171" s="11" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.45">
+        <v>621</v>
+      </c>
+      <c r="G171" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A172" s="1" t="s">
         <v>505</v>
       </c>
@@ -5791,8 +6881,11 @@
         <v>507</v>
       </c>
       <c r="E172" s="1"/>
-    </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G172" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A173" s="5" t="s">
         <v>508</v>
       </c>
@@ -5806,6 +6899,9 @@
         <v>510</v>
       </c>
       <c r="E173" s="5"/>
+      <c r="G173" t="s">
+        <v>510</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>